<commit_message>
Add conditional requirement validation
</commit_message>
<xml_diff>
--- a/openn/tests/data/diaries/bryn_mawr/HelenGriffith_Diary.xlsx
+++ b/openn/tests/data/diaries/bryn_mawr/HelenGriffith_Diary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="900" windowWidth="21840" windowHeight="19100"/>
+    <workbookView xWindow="20500" yWindow="0" windowWidth="20480" windowHeight="22580"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6255" uniqueCount="3977">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6244" uniqueCount="3968">
   <si>
     <t>1r</t>
   </si>
@@ -11071,57 +11071,6 @@
     <t>Volume number</t>
   </si>
   <si>
-    <t>altId</t>
-  </si>
-  <si>
-    <t>publisher</t>
-  </si>
-  <si>
-    <t>publisher/email</t>
-  </si>
-  <si>
-    <t>msIdentifier</t>
-  </si>
-  <si>
-    <t>titleStmt/title</t>
-  </si>
-  <si>
-    <t>titleStmt/author</t>
-  </si>
-  <si>
-    <t>origDate/@when</t>
-  </si>
-  <si>
-    <t>origDate/@from</t>
-  </si>
-  <si>
-    <t>origDate/@to</t>
-  </si>
-  <si>
-    <t>msContents/summary</t>
-  </si>
-  <si>
-    <t>msContents/textLang</t>
-  </si>
-  <si>
-    <t>msIdentifier/collection</t>
-  </si>
-  <si>
-    <t>notesStmt/note[@type=relatedResource]</t>
-  </si>
-  <si>
-    <t>notesStmt/note[@type=relatedResource]/@target</t>
-  </si>
-  <si>
-    <t>profileDesc/textClass/keywords[@n='subjects']/term</t>
-  </si>
-  <si>
-    <t>titleStmt/author/@ref</t>
-  </si>
-  <si>
-    <t>profileDesc/textClass/keywords[@n='form/genre']/term</t>
-  </si>
-  <si>
     <t>Subject: names URI [?]</t>
   </si>
   <si>
@@ -11134,9 +11083,6 @@
     <t>Subject: genre/form URI [?]</t>
   </si>
   <si>
-    <t>publicationStmt/availability/licence</t>
-  </si>
-  <si>
     <t>Rachel Appel</t>
   </si>
   <si>
@@ -11990,22 +11936,42 @@
   </si>
   <si>
     <t>XYZ ABC 1</t>
+  </si>
+  <si>
+    <t>Alternate ID</t>
+  </si>
+  <si>
+    <t>Alternate ID type</t>
+  </si>
+  <si>
+    <t>Date (narrative)</t>
+  </si>
+  <si>
+    <t>Place of origin</t>
+  </si>
+  <si>
+    <t>Number of physical pages</t>
+  </si>
+  <si>
+    <t>Gaps</t>
+  </si>
+  <si>
+    <t>Page dimensions</t>
+  </si>
+  <si>
+    <t>Bound dimensions</t>
+  </si>
+  <si>
+    <t>Bryn Mawr, Pennsylvania</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -12113,80 +12079,85 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="15" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="15" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="15" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="15" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="15" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="15" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="15" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -12207,6 +12178,12 @@
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -12528,104 +12505,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.6640625" style="6"/>
+    <col min="1" max="1" width="33.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="D1" s="6" t="s">
+    <row r="1" spans="1:22">
+      <c r="C1" s="6" t="s">
         <v>2630</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
-      <c r="D2" s="6" t="s">
+    <row r="2" spans="1:22">
+      <c r="C2" s="6" t="s">
         <v>2631</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
-      <c r="C6" s="5" t="s">
+    <row r="6" spans="1:22">
+      <c r="B6" s="5" t="s">
         <v>2632</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>2633</v>
+      </c>
       <c r="D6" s="4" t="s">
-        <v>2633</v>
+        <v>2634</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>2634</v>
+        <v>2635</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>2635</v>
+        <v>2636</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>2636</v>
+        <v>2637</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>2637</v>
+        <v>2638</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>2638</v>
+        <v>2639</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>2639</v>
+        <v>2640</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>2640</v>
+        <v>2641</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>2641</v>
+        <v>2642</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>2642</v>
+        <v>2643</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>2643</v>
+        <v>2644</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>2644</v>
+        <v>2645</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>2645</v>
+        <v>2646</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>2646</v>
+        <v>2647</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>2647</v>
+        <v>2648</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>2648</v>
+        <v>2649</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>2649</v>
+        <v>2650</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>2650</v>
+        <v>2651</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>2651</v>
-      </c>
-      <c r="W6" s="4" t="s">
         <v>2652</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="9" customFormat="1">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="1:22" s="9" customFormat="1">
+      <c r="A7" s="7" t="s">
         <v>2653</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -12645,18 +12622,18 @@
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="B8" s="4" t="s">
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="4" t="s">
         <v>2676</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>3692</v>
-      </c>
+      <c r="C8" s="4" t="s">
+        <v>3674</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -12675,18 +12652,18 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-    </row>
-    <row r="9" spans="1:23">
-      <c r="B9" s="4" t="s">
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="4" t="s">
         <v>2677</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>3693</v>
-      </c>
+      <c r="C9" s="18" t="s">
+        <v>3675</v>
+      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -12705,9 +12682,9 @@
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-    </row>
-    <row r="10" spans="1:23">
+    </row>
+    <row r="10" spans="1:22">
+      <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -12727,13 +12704,13 @@
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-    </row>
-    <row r="11" spans="1:23" s="9" customFormat="1">
-      <c r="B11" s="7" t="s">
+    </row>
+    <row r="11" spans="1:22" s="9" customFormat="1">
+      <c r="A11" s="7" t="s">
         <v>2654</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -12753,19 +12730,16 @@
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12" s="17" t="s">
-        <v>3670</v>
-      </c>
-      <c r="B12" s="4" t="s">
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="4" t="s">
         <v>3668</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -12784,40 +12758,39 @@
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="A13" s="17" t="s">
-        <v>3670</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>3669</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>2664</v>
-      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="4" t="s">
+        <v>2655</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>3676</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -12837,21 +12810,18 @@
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="A15" s="17" t="s">
-        <v>3671</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>2655</v>
-      </c>
-      <c r="C15" s="5" t="s">
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="4" t="s">
+        <v>2657</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>3694</v>
-      </c>
+      <c r="C15" s="18" t="s">
+        <v>3677</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -12870,54 +12840,48 @@
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-    </row>
-    <row r="16" spans="1:23">
-      <c r="A16" s="17" t="s">
-        <v>3672</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>2657</v>
-      </c>
-      <c r="C16" s="5" t="s">
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="4" t="s">
+        <v>2658</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>3695</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-    </row>
-    <row r="17" spans="1:23">
-      <c r="A17" s="17" t="s">
-        <v>3673</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>2658</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="C16" s="4" t="s">
+        <v>3678</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="4" t="s">
+        <v>2659</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>3696</v>
-      </c>
+      <c r="C17" s="4" t="s">
+        <v>3679</v>
+      </c>
+      <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -12936,203 +12900,170 @@
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-    </row>
-    <row r="18" spans="1:23">
-      <c r="A18" s="17" t="s">
-        <v>3673</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>2659</v>
-      </c>
-      <c r="C18" s="5" t="s">
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" s="4" t="s">
+        <v>2667</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>3842</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" s="4" t="s">
+        <v>2660</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>3697</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-    </row>
-    <row r="19" spans="1:23">
-      <c r="A19" s="17" t="s">
-        <v>3681</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>2667</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="20" t="s">
+        <v>3958</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" s="4" t="s">
+        <v>3959</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>3860</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23">
-      <c r="A20" s="17" t="s">
-        <v>3673</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>2660</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="4" t="s">
+        <v>3960</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>3657</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22" s="4" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>3976</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-    </row>
-    <row r="21" spans="1:23">
-      <c r="A21" s="17" t="s">
-        <v>3674</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>2661</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="C22" s="17" t="s">
+        <v>3923</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" s="4" t="s">
+        <v>3669</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="A24" s="4" t="s">
+        <v>2662</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>3941</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23">
-      <c r="A22" s="18" t="s">
-        <v>3675</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>2662</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>2656</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>3859</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23">
-      <c r="A23" s="18" t="s">
-        <v>3685</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="C24" s="17" t="s">
+        <v>3841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="A25" s="4" t="s">
         <v>2663</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="B25" s="5" t="s">
         <v>2664</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
-      <c r="A25" s="17" t="s">
-        <v>3676</v>
-      </c>
-      <c r="B25" s="4" t="s">
+    <row r="27" spans="1:22">
+      <c r="A27" s="4" t="s">
         <v>2680</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-    </row>
-    <row r="26" spans="1:23">
-      <c r="A26" s="17" t="s">
-        <v>3677</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>2681</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D26" s="20">
-        <v>1903</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-    </row>
-    <row r="27" spans="1:23">
-      <c r="A27" s="17" t="s">
-        <v>3678</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>2682</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D27" s="20">
-        <v>1909</v>
-      </c>
+      <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -13151,407 +13082,501 @@
       <c r="T27" s="11"/>
       <c r="U27" s="11"/>
       <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-    </row>
-    <row r="29" spans="1:23">
-      <c r="A29" s="17" t="s">
+    </row>
+    <row r="28" spans="1:22">
+      <c r="A28" s="4" t="s">
+        <v>2681</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C28" s="19">
+        <v>1903</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="A29" s="4" t="s">
+        <v>2682</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C29" s="19">
+        <v>1909</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="A30" s="4" t="s">
+        <v>3961</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31" s="4" t="s">
+        <v>3962</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>3967</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="4" t="s">
+        <v>2665</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>3957</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="4" t="s">
+        <v>2666</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="4" t="s">
+        <v>3963</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="4" t="s">
+        <v>3964</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="4" t="s">
+        <v>3965</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="4" t="s">
+        <v>3966</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="4" t="s">
+        <v>2678</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C41" s="17"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="4" t="s">
+        <v>2679</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="4" t="s">
+        <v>2668</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="4" t="s">
+        <v>3670</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="4" t="s">
+        <v>2669</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C47" s="17" t="s">
         <v>3679</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>2665</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="D47" s="17" t="s">
+        <v>3834</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>3835</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>3836</v>
+      </c>
+      <c r="G47" s="17"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="4" t="s">
+        <v>3671</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>2664</v>
       </c>
-      <c r="D29" s="18" t="s">
-        <v>3975</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23">
-      <c r="A30" s="17" t="s">
+      <c r="C48" s="6" t="s">
+        <v>3837</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>3838</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>3839</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22">
+      <c r="A50" s="4" t="s">
+        <v>2670</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>3680</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>2666</v>
-      </c>
-      <c r="C30" s="5" t="s">
+    </row>
+    <row r="51" spans="1:22">
+      <c r="A51" s="4" t="s">
+        <v>3672</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>3681</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
+      <c r="A53" s="4" t="s">
+        <v>2671</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>3682</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22">
+      <c r="A54" s="4" t="s">
+        <v>3673</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>2664</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>3683</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
+      <c r="A56" s="4" t="s">
+        <v>3661</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>2656</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>2935</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23">
-      <c r="A32" s="18" t="s">
-        <v>3682</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>2678</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D32" s="18"/>
-    </row>
-    <row r="33" spans="1:23">
-      <c r="A33" s="18" t="s">
-        <v>3683</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>2679</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>2664</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23">
-      <c r="A35" s="18" t="s">
+      <c r="C56" s="17" t="s">
+        <v>2672</v>
+      </c>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+    </row>
+    <row r="57" spans="1:22">
+      <c r="A57" s="4" t="s">
+        <v>3656</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>3657</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="11"/>
+      <c r="T57" s="11"/>
+      <c r="U57" s="11"/>
+      <c r="V57" s="11"/>
+    </row>
+    <row r="58" spans="1:22">
+      <c r="A58" s="4" t="s">
+        <v>3658</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>3657</v>
+      </c>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="11"/>
+      <c r="T58" s="11"/>
+      <c r="U58" s="11"/>
+      <c r="V58" s="11"/>
+    </row>
+    <row r="60" spans="1:22">
+      <c r="A60" s="4" t="s">
+        <v>3662</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>2656</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>2674</v>
+      </c>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="T60" s="11"/>
+      <c r="U60" s="11"/>
+      <c r="V60" s="11"/>
+    </row>
+    <row r="61" spans="1:22">
+      <c r="A61" s="4" t="s">
+        <v>3659</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>3657</v>
+      </c>
+      <c r="C61" s="17" t="s">
         <v>3684</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>2668</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-    </row>
-    <row r="36" spans="1:23">
-      <c r="B36" s="4" t="s">
-        <v>3687</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>2664</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23">
-      <c r="A38" s="18" t="s">
-        <v>3684</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>2669</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>3697</v>
-      </c>
-      <c r="E38" s="18" t="s">
-        <v>3852</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>3853</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>3854</v>
-      </c>
-      <c r="H38" s="18"/>
-    </row>
-    <row r="39" spans="1:23">
-      <c r="B39" s="4" t="s">
-        <v>3688</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>3855</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>3856</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>3857</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>3858</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23">
-      <c r="A41" s="18" t="s">
-        <v>3684</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>2670</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>3698</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23">
-      <c r="B42" s="4" t="s">
-        <v>3689</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>3699</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23">
-      <c r="A44" s="18" t="s">
-        <v>3686</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>2671</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>3700</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23">
-      <c r="A45" s="18"/>
-      <c r="B45" s="4" t="s">
-        <v>3690</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>2664</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>3701</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23">
-      <c r="A47" s="18" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>3661</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>2656</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>2672</v>
-      </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="11"/>
-      <c r="U47" s="11"/>
-      <c r="V47" s="11"/>
-      <c r="W47" s="11"/>
-    </row>
-    <row r="48" spans="1:23">
-      <c r="A48" s="18" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>3656</v>
-      </c>
-      <c r="C48" s="5" t="s">
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="K61" s="11"/>
+      <c r="L61" s="11"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="11"/>
+      <c r="O61" s="11"/>
+      <c r="P61" s="11"/>
+      <c r="Q61" s="11"/>
+      <c r="R61" s="11"/>
+      <c r="S61" s="11"/>
+      <c r="T61" s="11"/>
+      <c r="U61" s="11"/>
+      <c r="V61" s="11"/>
+    </row>
+    <row r="62" spans="1:22">
+      <c r="A62" s="4" t="s">
+        <v>3660</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>3657</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
-      <c r="T48" s="11"/>
-      <c r="U48" s="11"/>
-      <c r="V48" s="11"/>
-      <c r="W48" s="11"/>
-    </row>
-    <row r="49" spans="1:23">
-      <c r="A49" s="18" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>3658</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>3657</v>
-      </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
-      <c r="V49" s="11"/>
-      <c r="W49" s="11"/>
-    </row>
-    <row r="51" spans="1:23">
-      <c r="A51" s="18" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>3662</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>2656</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>2674</v>
-      </c>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
-      <c r="T51" s="11"/>
-      <c r="U51" s="11"/>
-      <c r="V51" s="11"/>
-      <c r="W51" s="11"/>
-    </row>
-    <row r="52" spans="1:23">
-      <c r="A52" s="18" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>3659</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>3657</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>3702</v>
-      </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-      <c r="S52" s="11"/>
-      <c r="T52" s="11"/>
-      <c r="U52" s="11"/>
-      <c r="V52" s="11"/>
-      <c r="W52" s="11"/>
-    </row>
-    <row r="53" spans="1:23">
-      <c r="A53" s="18" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>3660</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>3657</v>
-      </c>
-      <c r="D53" s="6">
+      <c r="C62" s="6">
         <v>2012</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-      <c r="S53" s="11"/>
-      <c r="T53" s="11"/>
-      <c r="U53" s="11"/>
-      <c r="V53" s="11"/>
-      <c r="W53" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11"/>
+      <c r="L62" s="11"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="11"/>
+      <c r="O62" s="11"/>
+      <c r="P62" s="11"/>
+      <c r="Q62" s="11"/>
+      <c r="R62" s="11"/>
+      <c r="S62" s="11"/>
+      <c r="T62" s="11"/>
+      <c r="U62" s="11"/>
+      <c r="V62" s="11"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="298" yWindow="489" count="21">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source URL" prompt="[Optional; multiple values]_x000d__x000d_URL for a finding aid or catalog record for the manuscript." sqref="D33"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Language" prompt="[Required; multiple values]_x000d__x000d_One or more language codes for the manuscript content. Use ISO-539-2 http://www.loc.gov/standards/iso639-2/php/code_list.php. Use bibliographic code rather than terminology code when applicable. " sqref="D30"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="[Optional; single value]_x000d__x000d_From 520 and 545 of catalog record; or biog/hist and scope and contents notes of finding aids. Suggested limit: 1000 words for both 520 and 545 notes combined." sqref="D29"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date" prompt="[Required; one value per field]_x000d__x000d_Date or dates of mansucript creation. A single year, 'Date when' , or a range expressed by two years, 'Date start' and 'Date end'." sqref="D25"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creator URI" prompt="[Optional; multiple values]_x000d__x000d_If available, URI to authority record for the above named author (e.g., VIAF or LCNAF)." sqref="D23:D24"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creator name" prompt="[Required; multiple values]_x000d__x000d_Either (1) the name(s) of manuscript's author(s), (2) Anonymous, or (3) Unknown. When an author name cannot be given, use 'Anonymous' for authors who intentionally do not reveal identity and 'Unknown' otherwise." sqref="D22"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Title" prompt="[Required; multiple values]_x000d__x000d_A title for the manuscript, either a formal title or one devised for the manuscript. Ideally, title should conform with the recommendation in DACS (Describing Archives: A Content Standard). Alternate titles may be provided. " sqref="D21"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository name" prompt="[Required; multiple values]_x000d__x000d_Manuscript identifier, like call number. List primary identifier first. " sqref="D20"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository name" prompt="[Required; single value]_x000d__x000d_Repository where the manuscript is kept. " sqref="D18"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository City" prompt="[Required; single value]_x000d__x000d_City of the repository where the manuscript is kept. " sqref="D17"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata creator email" prompt="Contact email for above named metadata creator." sqref="D16"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata creator" prompt="The individual or organization responsible for the creation of this metadata record. One name per column." sqref="D15"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Administrative contact" prompt="[Required; multiple values]_x000d__x000d_Person or persons to contact with problems or questions about this metadata of these files during processing._x000d__x000d_THIS VALUE IS NOT FOR PUBLICATION." sqref="D8"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Administrative contact email" prompt="[Required; multiple values]_x000d__x000d_Email address of the above-named person._x000d__x000d_THIS VALUE IS NOT FOR PUBLICATION." sqref="D9"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright holder" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Image rights&quot; is CC0 or CC-BY._x000d__x000d_Copyright does not apply to public domain material._x000d_ _x000d_" sqref="D48"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright year" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Image rights&quot; is CC0 or CC-BY. _x000d__x000d_Copyright does not apply to public domain material._x000d__x000d_The year of the images' copyright. Current year will be used by default if &quot;Image rights&quot; is CC0 or CC-BY._x000d_" sqref="D49">
+  <dataValidations xWindow="298" yWindow="489" count="29">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source URL" prompt="[Optional; multiple values]_x000d__x000d_URL for a finding aid or catalog record for the manuscript." sqref="C42"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Language" prompt="[Required; multiple values]_x000d__x000d_One or more language codes for the manuscript content. Use ISO-539-2 http://www.loc.gov/standards/iso639-2/php/code_list.php. Use bibliographic code rather than terminology code when applicable. " sqref="C34"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Description" prompt="[Optional; single value]_x000d__x000d_From 520 and 545 of catalog record; or biog/hist and scope and contents notes of finding aids. Suggested limit: 1000 words for both 520 and 545 notes combined." sqref="C33"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date" prompt="[Required; one value per field]_x000d__x000d_Date or dates of mansucript creation. A single year, 'Date when' , or a range expressed by two years, 'Date start' and 'Date end'." sqref="C27"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creator URI" prompt="[Optional; multiple values]_x000d__x000d_If available, URI to authority record for the above named author (e.g., VIAF or LCNAF)." sqref="C25:C26"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Creator name" prompt="[Required; multiple values]_x000d__x000d_Either (1) the name(s) of manuscript's author(s), (2) Anonymous, or (3) Unknown. When an author name cannot be given, use 'Anonymous' for authors who intentionally do not reveal identity and 'Unknown' otherwise." sqref="C24"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Title" prompt="[Required; multiple values]_x000d__x000d_A title for the manuscript, either a formal title or one devised for the manuscript. Ideally, title should conform with the recommendation in DACS (Describing Archives: A Content Standard). Alternate titles may be provided. " sqref="C22"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository name" prompt="[Required; multiple values]_x000d__x000d_Manuscript identifier, like call number. List primary identifier first. " sqref="C19"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository name" prompt="[Required; single value]_x000d__x000d_Repository where the manuscript is kept. " sqref="C17"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Repository City" prompt="[Required; single value]_x000d__x000d_City of the repository where the manuscript is kept. " sqref="C16"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata creator email" prompt="Contact email for above named metadata creator." sqref="C15"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata creator" prompt="The individual or organization responsible for the creation of this metadata record. One name per column." sqref="C14"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Administrative contact" prompt="[Required; multiple values]_x000d__x000d_Person or persons to contact with problems or questions about this metadata of these files during processing._x000d__x000d_THIS VALUE IS NOT FOR PUBLICATION." sqref="C8"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Administrative contact email" prompt="[Required; multiple values]_x000d__x000d_Email address of the above-named person._x000d__x000d_THIS VALUE IS NOT FOR PUBLICATION." sqref="C9"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright holder" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Image rights&quot; is CC0 or CC-BY._x000d__x000d_Copyright does not apply to public domain material._x000d_ _x000d_" sqref="C57"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright year" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Image rights&quot; is CC0 or CC-BY. _x000d__x000d_Copyright does not apply to public domain material._x000d__x000d_The year of the images' copyright. Current year will be used by default if &quot;Image rights&quot; is CC0 or CC-BY._x000d_" sqref="C58">
       <formula1>1800</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright holder" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Metadata rights&quot; is CC0 or CC-BY._x000d__x000d_Copyright does not apply to public domain material._x000d_ _x000d_" sqref="D52"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright year" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Metadata rights&quot; is CC0 or CC-BY.  Copyright does not apply to public domain material._x000d__x000d_The year of the metadata's copyright. Current year will be used by default if &quot;Metada rights&quot; is CC0 or CC-BY." sqref="D53">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright holder" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Metadata rights&quot; is CC0 or CC-BY._x000d__x000d_Copyright does not apply to public domain material._x000d_ _x000d_" sqref="C61"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter copyright year" prompt="[Conditionally required; single value]_x000d__x000d_Fill in only if &quot;Metadata rights&quot; is CC0 or CC-BY.  Copyright does not apply to public domain material._x000d__x000d_The year of the metadata's copyright. Current year will be used by default if &quot;Metada rights&quot; is CC0 or CC-BY." sqref="C62">
       <formula1>1800</formula1>
       <formula2>2100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter PACSCL Diaires Project ID" prompt="[required; single value]_x000d__x000d_This is the number that was provided to you for this diary, a number like 'PDP001', 'PDP002', etc." sqref="D12"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter Volume number" prompt="[reqiued for multi-volume objects; single value]_x000d__x000d_If a multi-volume work, enter a whole number volume here. This value is used for database sorting._x000d__x000d_Complex or non-numeric volume numbers, like 'Volume A' or 'Vol. IV', should be added to the volume title." sqref="D13">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter PACSCL Diaires Project ID" prompt="[required; single value]_x000d__x000d_This is the number that was provided to you for this diary, a number like 'PDP001', 'PDP002', etc." sqref="C12"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Enter Volume number" prompt="[reqiued for multi-volume objects; single value]_x000d__x000d_If a multi-volume work, enter a whole number volume here. This value is used for database sorting._x000d__x000d_Complex or non-numeric volume numbers, like 'Volume A' or 'Vol. IV', should be added to the volume title." sqref="C23">
       <formula1>1</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source" prompt="[Optional; multiple value]_x000d__x000d_Name of a larger collection to which this manuscript belongs." sqref="D19 D31:D32"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Source" prompt="[Optional; multiple value]_x000d__x000d_Name of a larger collection to which this manuscript belongs." sqref="C18 C35 C40:C41"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Alternate ID" prompt="[Optional; single value]_x000d__x000d_In addition to a call number, one alternate identifier may be given. This can be an internal control number or URN, such as DOI, PURL, or ARK._x000d__x000d_An ID that is part of a persistent URL should be given in URL form." sqref="C20"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Alternate ID Type" prompt="[required if alternate ID provided; single value]_x000d__x000d_The type of Alternate ID above, if entered; e.g., DOI, ARK, PURL, or BibID." sqref="C21"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Date (narrative)" prompt="[Optional; single value]_x000d__x000d_Text description of date of origin for document. If blank, narrative will be built from year values._x000d__x000d_Examples: &quot;Late 19th C.&quot;; &quot;May 3, 1902 to January 26, 1914&quot;; &quot;Main text written in 1872, with annotations added in 1940&quot;" sqref="C30"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Place of origin" prompt="[Required; multiple values]_x000d__x000d_One or more places of origin for this document; if not known, use &quot;Unknown&quot;. Historical or modern place names may be used." sqref="C31"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Bound dimensions" prompt="[Optional; single value]_x000d__x000d_Height and width of the bound document in millimeters._x000d__x000d_Example: &quot;215 x 162 mm&quot;" sqref="C39"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Page dimensions" prompt="[Optional; single value]_x000d__x000d_Height and width of a document page in millimeters._x000d__x000d_Example: &quot;205 x 150 mm&quot;" sqref="C38"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Gaps" prompt="[Optional; single value]_x000d__x000d_Description of pages not imaged or physical pages missing from the document itself. _x000d__x000d_Example: &quot;Blank pages 230-250 were not imaged&quot;; &quot;Folio 23 missing from manuscript.&quot;" sqref="C37"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Number of physical pages" prompt="[Optional; single value]_x000d__x000d_Text describing the number of pages in this document. " sqref="C36"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
-    <hyperlink ref="D16" r:id="rId2"/>
-    <hyperlink ref="D45" r:id="rId3"/>
+    <hyperlink ref="C9" r:id="rId1"/>
+    <hyperlink ref="C15" r:id="rId2"/>
+    <hyperlink ref="C54" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -13562,13 +13587,13 @@
           <x14:formula1>
             <xm:f>'VALUE LISTS'!$D$3:$D$12</xm:f>
           </x14:formula1>
-          <xm:sqref>D47</xm:sqref>
+          <xm:sqref>C56</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select metadata licence" prompt="[Required; single value]_x000d__x000d_PD - metadata in Public Domain_x000d__x000d_CC0 - &quot;CC zero&quot;; metadata copyrighted but released to Public Domain_x000d__x000d_CC-BY - metadata released with Creative Commons Attribution License">
           <x14:formula1>
             <xm:f>'VALUE LISTS'!$D$3:$D$12</xm:f>
           </x14:formula1>
-          <xm:sqref>D51</xm:sqref>
+          <xm:sqref>C60</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -13662,13 +13687,13 @@
         <v>2601</v>
       </c>
       <c r="D4" t="s">
-        <v>3861</v>
+        <v>3843</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>2620</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>3703</v>
+        <v>3685</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -13679,13 +13704,13 @@
         <v>2602</v>
       </c>
       <c r="D5" t="s">
-        <v>3862</v>
+        <v>3844</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>3704</v>
+        <v>3686</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -13696,13 +13721,13 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>3863</v>
+        <v>3845</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>3705</v>
+        <v>3687</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -13713,19 +13738,19 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>3864</v>
+        <v>3846</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>3706</v>
+        <v>3688</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>3707</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -13736,19 +13761,19 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>3865</v>
+        <v>3847</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>3708</v>
+        <v>3690</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>3709</v>
+        <v>3691</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -13759,19 +13784,19 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>3866</v>
+        <v>3848</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>3710</v>
+        <v>3692</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>3711</v>
+        <v>3693</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -13782,19 +13807,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>3867</v>
+        <v>3849</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>3713</v>
+        <v>3695</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>3712</v>
+        <v>3694</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -13805,19 +13830,19 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>3868</v>
+        <v>3850</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>3714</v>
+        <v>3696</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>3715</v>
+        <v>3697</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -13828,19 +13853,19 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>3869</v>
+        <v>3851</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>3716</v>
+        <v>3698</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>3717</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -13851,19 +13876,19 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>3870</v>
+        <v>3852</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>3718</v>
+        <v>3700</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>3719</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -13874,25 +13899,25 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>3871</v>
+        <v>3853</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>3720</v>
+        <v>3702</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>3721</v>
+        <v>3703</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>3722</v>
+        <v>3704</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -13903,25 +13928,25 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>3872</v>
+        <v>3854</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>3723</v>
+        <v>3705</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>3724</v>
+        <v>3706</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>3725</v>
+        <v>3707</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -13932,19 +13957,19 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>3873</v>
+        <v>3855</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>3713</v>
+        <v>3695</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>3726</v>
+        <v>3708</v>
       </c>
     </row>
     <row r="17" spans="2:10">
@@ -13955,25 +13980,25 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>3874</v>
+        <v>3856</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>3727</v>
+        <v>3709</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>3728</v>
+        <v>3710</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>3729</v>
+        <v>3711</v>
       </c>
     </row>
     <row r="18" spans="2:10">
@@ -13984,19 +14009,19 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>3875</v>
+        <v>3857</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>3730</v>
+        <v>3712</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>3731</v>
+        <v>3713</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -14007,19 +14032,19 @@
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>3876</v>
+        <v>3858</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>3732</v>
+        <v>3714</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>3733</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="20" spans="2:10">
@@ -14030,19 +14055,19 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>3877</v>
+        <v>3859</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>3734</v>
+        <v>3716</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>3735</v>
+        <v>3717</v>
       </c>
     </row>
     <row r="21" spans="2:10">
@@ -14053,19 +14078,19 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>3878</v>
+        <v>3860</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>3736</v>
+        <v>3718</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>3737</v>
+        <v>3719</v>
       </c>
     </row>
     <row r="22" spans="2:10">
@@ -14076,19 +14101,19 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>3879</v>
+        <v>3861</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>3738</v>
+        <v>3720</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>3739</v>
+        <v>3721</v>
       </c>
     </row>
     <row r="23" spans="2:10">
@@ -14099,25 +14124,25 @@
         <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>3880</v>
+        <v>3862</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>3740</v>
+        <v>3722</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>3741</v>
+        <v>3723</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>3742</v>
+        <v>3724</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -14128,13 +14153,13 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>3881</v>
+        <v>3863</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>3743</v>
+        <v>3725</v>
       </c>
     </row>
     <row r="25" spans="2:10">
@@ -14145,19 +14170,19 @@
         <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>3882</v>
+        <v>3864</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>3744</v>
+        <v>3726</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>3745</v>
+        <v>3727</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -14168,19 +14193,19 @@
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>3883</v>
+        <v>3865</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>3746</v>
+        <v>3728</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H26" s="15" t="s">
-        <v>3747</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="27" spans="2:10">
@@ -14191,19 +14216,19 @@
         <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>3884</v>
+        <v>3866</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>3748</v>
+        <v>3730</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>3749</v>
+        <v>3731</v>
       </c>
     </row>
     <row r="28" spans="2:10">
@@ -14214,19 +14239,19 @@
         <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>3885</v>
+        <v>3867</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>3750</v>
+        <v>3732</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H28" s="15" t="s">
-        <v>3751</v>
+        <v>3733</v>
       </c>
     </row>
     <row r="29" spans="2:10">
@@ -14237,19 +14262,19 @@
         <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>3886</v>
+        <v>3868</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>3752</v>
+        <v>3734</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H29" s="15" t="s">
-        <v>3753</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="30" spans="2:10">
@@ -14260,19 +14285,19 @@
         <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>3887</v>
+        <v>3869</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>3754</v>
+        <v>3736</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>3755</v>
+        <v>3737</v>
       </c>
     </row>
     <row r="31" spans="2:10">
@@ -14283,19 +14308,19 @@
         <v>25</v>
       </c>
       <c r="D31" t="s">
-        <v>3888</v>
+        <v>3870</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>3756</v>
+        <v>3738</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H31" s="15" t="s">
-        <v>3757</v>
+        <v>3739</v>
       </c>
     </row>
     <row r="32" spans="2:10">
@@ -14306,19 +14331,19 @@
         <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>3889</v>
+        <v>3871</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>3758</v>
+        <v>3740</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>3759</v>
+        <v>3741</v>
       </c>
     </row>
     <row r="33" spans="2:10">
@@ -14329,19 +14354,19 @@
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>3890</v>
+        <v>3872</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>3760</v>
+        <v>3742</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>3761</v>
+        <v>3743</v>
       </c>
     </row>
     <row r="34" spans="2:10">
@@ -14352,19 +14377,19 @@
         <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>3891</v>
+        <v>3873</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>3762</v>
+        <v>3744</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>3763</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="35" spans="2:10">
@@ -14375,19 +14400,19 @@
         <v>29</v>
       </c>
       <c r="D35" t="s">
-        <v>3892</v>
+        <v>3874</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>3764</v>
+        <v>3746</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>3765</v>
+        <v>3747</v>
       </c>
     </row>
     <row r="36" spans="2:10">
@@ -14398,19 +14423,19 @@
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>3893</v>
+        <v>3875</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>3766</v>
+        <v>3748</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>3767</v>
+        <v>3749</v>
       </c>
     </row>
     <row r="37" spans="2:10">
@@ -14421,13 +14446,13 @@
         <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>3894</v>
+        <v>3876</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>3768</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="38" spans="2:10">
@@ -14438,25 +14463,25 @@
         <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>3895</v>
+        <v>3877</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>3769</v>
+        <v>3751</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>3770</v>
+        <v>3752</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>3771</v>
+        <v>3753</v>
       </c>
     </row>
     <row r="39" spans="2:10">
@@ -14467,19 +14492,19 @@
         <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>3896</v>
+        <v>3878</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>3773</v>
+        <v>3755</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H39" s="15" t="s">
-        <v>3774</v>
+        <v>3756</v>
       </c>
     </row>
     <row r="40" spans="2:10">
@@ -14490,13 +14515,13 @@
         <v>34</v>
       </c>
       <c r="D40" t="s">
-        <v>3897</v>
+        <v>3879</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>3772</v>
+        <v>3754</v>
       </c>
     </row>
     <row r="41" spans="2:10">
@@ -14507,13 +14532,13 @@
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>3898</v>
+        <v>3880</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>3775</v>
+        <v>3757</v>
       </c>
     </row>
     <row r="42" spans="2:10">
@@ -14524,25 +14549,25 @@
         <v>36</v>
       </c>
       <c r="D42" t="s">
-        <v>3899</v>
+        <v>3881</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>3776</v>
+        <v>3758</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>3777</v>
+        <v>3759</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J42" s="15" t="s">
-        <v>3778</v>
+        <v>3760</v>
       </c>
     </row>
     <row r="43" spans="2:10">
@@ -14553,25 +14578,25 @@
         <v>37</v>
       </c>
       <c r="D43" t="s">
-        <v>3900</v>
+        <v>3882</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>3779</v>
+        <v>3761</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>3780</v>
+        <v>3762</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J43" s="15" t="s">
-        <v>3781</v>
+        <v>3763</v>
       </c>
     </row>
     <row r="44" spans="2:10">
@@ -14582,19 +14607,19 @@
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>3901</v>
+        <v>3883</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>3782</v>
+        <v>3764</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>3783</v>
+        <v>3765</v>
       </c>
     </row>
     <row r="45" spans="2:10">
@@ -14605,25 +14630,25 @@
         <v>39</v>
       </c>
       <c r="D45" t="s">
-        <v>3902</v>
+        <v>3884</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>3784</v>
+        <v>3766</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>3785</v>
+        <v>3767</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="J45" s="15" t="s">
-        <v>3786</v>
+        <v>3768</v>
       </c>
     </row>
     <row r="46" spans="2:10">
@@ -14634,19 +14659,19 @@
         <v>40</v>
       </c>
       <c r="D46" t="s">
-        <v>3903</v>
+        <v>3885</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>3787</v>
+        <v>3769</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>3788</v>
+        <v>3770</v>
       </c>
     </row>
     <row r="47" spans="2:10">
@@ -14657,25 +14682,25 @@
         <v>41</v>
       </c>
       <c r="D47" t="s">
-        <v>3904</v>
+        <v>3886</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>3789</v>
+        <v>3771</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>3790</v>
+        <v>3772</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J47" s="15" t="s">
-        <v>3791</v>
+        <v>3773</v>
       </c>
     </row>
     <row r="48" spans="2:10">
@@ -14686,19 +14711,19 @@
         <v>42</v>
       </c>
       <c r="D48" t="s">
-        <v>3905</v>
+        <v>3887</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>3792</v>
+        <v>3774</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>3794</v>
+        <v>3776</v>
       </c>
     </row>
     <row r="49" spans="2:10">
@@ -14709,19 +14734,19 @@
         <v>43</v>
       </c>
       <c r="D49" t="s">
-        <v>3906</v>
+        <v>3888</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>3795</v>
+        <v>3777</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>3796</v>
+        <v>3778</v>
       </c>
     </row>
     <row r="50" spans="2:10">
@@ -14732,19 +14757,19 @@
         <v>44</v>
       </c>
       <c r="D50" t="s">
-        <v>3907</v>
+        <v>3889</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>3797</v>
+        <v>3779</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>3798</v>
+        <v>3780</v>
       </c>
     </row>
     <row r="51" spans="2:10">
@@ -14755,19 +14780,19 @@
         <v>45</v>
       </c>
       <c r="D51" t="s">
-        <v>3908</v>
+        <v>3890</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>3793</v>
+        <v>3775</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>3799</v>
+        <v>3781</v>
       </c>
     </row>
     <row r="52" spans="2:10">
@@ -14778,19 +14803,19 @@
         <v>46</v>
       </c>
       <c r="D52" t="s">
-        <v>3909</v>
+        <v>3891</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>3800</v>
+        <v>3782</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>3801</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="53" spans="2:10">
@@ -14801,19 +14826,19 @@
         <v>47</v>
       </c>
       <c r="D53" t="s">
-        <v>3910</v>
+        <v>3892</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>3802</v>
+        <v>3784</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>3803</v>
+        <v>3785</v>
       </c>
     </row>
     <row r="54" spans="2:10">
@@ -14824,19 +14849,19 @@
         <v>48</v>
       </c>
       <c r="D54" t="s">
-        <v>3911</v>
+        <v>3893</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>3804</v>
+        <v>3786</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>3805</v>
+        <v>3787</v>
       </c>
     </row>
     <row r="55" spans="2:10">
@@ -14847,19 +14872,19 @@
         <v>49</v>
       </c>
       <c r="D55" t="s">
-        <v>3912</v>
+        <v>3894</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>3806</v>
+        <v>3788</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>3807</v>
+        <v>3789</v>
       </c>
     </row>
     <row r="56" spans="2:10">
@@ -14870,19 +14895,19 @@
         <v>50</v>
       </c>
       <c r="D56" t="s">
-        <v>3913</v>
+        <v>3895</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>3808</v>
+        <v>3790</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>3809</v>
+        <v>3791</v>
       </c>
     </row>
     <row r="57" spans="2:10">
@@ -14893,19 +14918,19 @@
         <v>51</v>
       </c>
       <c r="D57" t="s">
-        <v>3914</v>
+        <v>3896</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>3810</v>
+        <v>3792</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>3811</v>
+        <v>3793</v>
       </c>
     </row>
     <row r="58" spans="2:10">
@@ -14916,25 +14941,25 @@
         <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>3915</v>
+        <v>3897</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>3812</v>
+        <v>3794</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>3813</v>
+        <v>3795</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J58" s="15" t="s">
-        <v>3775</v>
+        <v>3757</v>
       </c>
     </row>
     <row r="59" spans="2:10">
@@ -14945,25 +14970,25 @@
         <v>53</v>
       </c>
       <c r="D59" t="s">
-        <v>3916</v>
+        <v>3898</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>3814</v>
+        <v>3796</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>3815</v>
+        <v>3797</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J59" s="15" t="s">
-        <v>3816</v>
+        <v>3798</v>
       </c>
     </row>
     <row r="60" spans="2:10">
@@ -14974,25 +14999,25 @@
         <v>54</v>
       </c>
       <c r="D60" t="s">
-        <v>3917</v>
+        <v>3899</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>3817</v>
+        <v>3799</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>3818</v>
+        <v>3800</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J60" s="15" t="s">
-        <v>3819</v>
+        <v>3801</v>
       </c>
     </row>
     <row r="61" spans="2:10">
@@ -15003,13 +15028,13 @@
         <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>3918</v>
+        <v>3900</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>3820</v>
+        <v>3802</v>
       </c>
     </row>
     <row r="62" spans="2:10">
@@ -15020,19 +15045,19 @@
         <v>56</v>
       </c>
       <c r="D62" t="s">
-        <v>3919</v>
+        <v>3901</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>3713</v>
+        <v>3695</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>3821</v>
+        <v>3803</v>
       </c>
     </row>
     <row r="63" spans="2:10">
@@ -15043,19 +15068,19 @@
         <v>57</v>
       </c>
       <c r="D63" t="s">
-        <v>3920</v>
+        <v>3902</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>3822</v>
+        <v>3804</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>3823</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="64" spans="2:10">
@@ -15066,19 +15091,19 @@
         <v>58</v>
       </c>
       <c r="D64" t="s">
-        <v>3921</v>
+        <v>3903</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>3824</v>
+        <v>3806</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>3825</v>
+        <v>3807</v>
       </c>
     </row>
     <row r="65" spans="2:12">
@@ -15089,19 +15114,19 @@
         <v>59</v>
       </c>
       <c r="D65" t="s">
-        <v>3922</v>
+        <v>3904</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>3826</v>
+        <v>3808</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>3827</v>
+        <v>3809</v>
       </c>
     </row>
     <row r="66" spans="2:12">
@@ -15112,19 +15137,19 @@
         <v>60</v>
       </c>
       <c r="D66" t="s">
-        <v>3923</v>
+        <v>3905</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>3828</v>
+        <v>3810</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>3829</v>
+        <v>3811</v>
       </c>
     </row>
     <row r="67" spans="2:12">
@@ -15135,19 +15160,19 @@
         <v>61</v>
       </c>
       <c r="D67" t="s">
-        <v>3924</v>
+        <v>3906</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>3830</v>
+        <v>3812</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>3715</v>
+        <v>3697</v>
       </c>
     </row>
     <row r="68" spans="2:12">
@@ -15158,19 +15183,19 @@
         <v>62</v>
       </c>
       <c r="D68" t="s">
-        <v>3925</v>
+        <v>3907</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>3716</v>
+        <v>3698</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>3717</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="69" spans="2:12">
@@ -15181,19 +15206,19 @@
         <v>63</v>
       </c>
       <c r="D69" t="s">
-        <v>3926</v>
+        <v>3908</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>3718</v>
+        <v>3700</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>3719</v>
+        <v>3701</v>
       </c>
     </row>
     <row r="70" spans="2:12">
@@ -15204,31 +15229,31 @@
         <v>64</v>
       </c>
       <c r="D70" t="s">
-        <v>3927</v>
+        <v>3909</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F70" s="15" t="s">
-        <v>3720</v>
+        <v>3702</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>3831</v>
+        <v>3813</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="J70" s="15" t="s">
-        <v>3720</v>
+        <v>3702</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="L70" s="15" t="s">
-        <v>3831</v>
+        <v>3813</v>
       </c>
     </row>
     <row r="71" spans="2:12">
@@ -15239,19 +15264,19 @@
         <v>65</v>
       </c>
       <c r="D71" t="s">
-        <v>3928</v>
+        <v>3910</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>3832</v>
+        <v>3814</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>3721</v>
+        <v>3703</v>
       </c>
     </row>
     <row r="72" spans="2:12">
@@ -15262,19 +15287,19 @@
         <v>66</v>
       </c>
       <c r="D72" t="s">
-        <v>3929</v>
+        <v>3911</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="F72" s="15" t="s">
-        <v>3713</v>
+        <v>3695</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>3833</v>
+        <v>3815</v>
       </c>
     </row>
     <row r="73" spans="2:12">
@@ -15285,19 +15310,19 @@
         <v>67</v>
       </c>
       <c r="D73" t="s">
-        <v>3930</v>
+        <v>3912</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>3713</v>
+        <v>3695</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>3834</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="74" spans="2:12">
@@ -15308,19 +15333,19 @@
         <v>68</v>
       </c>
       <c r="D74" t="s">
-        <v>3931</v>
+        <v>3913</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="F74" s="15" t="s">
-        <v>3713</v>
+        <v>3695</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>3835</v>
+        <v>3817</v>
       </c>
     </row>
     <row r="75" spans="2:12">
@@ -15331,19 +15356,19 @@
         <v>69</v>
       </c>
       <c r="D75" t="s">
-        <v>3932</v>
+        <v>3914</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>3713</v>
+        <v>3695</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>3836</v>
+        <v>3818</v>
       </c>
     </row>
     <row r="76" spans="2:12">
@@ -15354,19 +15379,19 @@
         <v>70</v>
       </c>
       <c r="D76" t="s">
-        <v>3933</v>
+        <v>3915</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>3667</v>
       </c>
       <c r="F76" s="15" t="s">
-        <v>3713</v>
+        <v>3695</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>3837</v>
+        <v>3819</v>
       </c>
     </row>
     <row r="77" spans="2:12">
@@ -15377,25 +15402,25 @@
         <v>71</v>
       </c>
       <c r="D77" t="s">
-        <v>3934</v>
+        <v>3916</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>3838</v>
+        <v>3820</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="H77" s="15" t="s">
-        <v>3839</v>
+        <v>3821</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J77" s="15" t="s">
-        <v>3840</v>
+        <v>3822</v>
       </c>
     </row>
     <row r="78" spans="2:12">
@@ -15406,25 +15431,25 @@
         <v>72</v>
       </c>
       <c r="D78" t="s">
-        <v>3935</v>
+        <v>3917</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F78" s="15" t="s">
-        <v>3841</v>
+        <v>3823</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>3842</v>
+        <v>3824</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J78" s="15" t="s">
-        <v>3843</v>
+        <v>3825</v>
       </c>
     </row>
     <row r="79" spans="2:12">
@@ -15435,19 +15460,19 @@
         <v>73</v>
       </c>
       <c r="D79" t="s">
-        <v>3936</v>
+        <v>3918</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>3844</v>
+        <v>3826</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>3845</v>
+        <v>3827</v>
       </c>
     </row>
     <row r="80" spans="2:12">
@@ -15458,25 +15483,25 @@
         <v>74</v>
       </c>
       <c r="D80" t="s">
-        <v>3937</v>
+        <v>3919</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>3846</v>
+        <v>3828</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>3711</v>
+        <v>3693</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J80" s="15" t="s">
-        <v>3834</v>
+        <v>3816</v>
       </c>
     </row>
     <row r="81" spans="2:12">
@@ -15487,31 +15512,31 @@
         <v>75</v>
       </c>
       <c r="D81" t="s">
-        <v>3938</v>
+        <v>3920</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F81" s="15" t="s">
-        <v>3835</v>
+        <v>3817</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>3847</v>
+        <v>3829</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J81" s="15" t="s">
-        <v>3731</v>
+        <v>3713</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>2620</v>
       </c>
       <c r="L81" s="15" t="s">
-        <v>3848</v>
+        <v>3830</v>
       </c>
     </row>
     <row r="82" spans="2:12">
@@ -15522,25 +15547,25 @@
         <v>76</v>
       </c>
       <c r="D82" t="s">
-        <v>3939</v>
+        <v>3921</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F82" s="15" t="s">
-        <v>3732</v>
+        <v>3714</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>3733</v>
+        <v>3715</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J82" s="15" t="s">
-        <v>3734</v>
+        <v>3716</v>
       </c>
     </row>
     <row r="83" spans="2:12">
@@ -15551,25 +15576,25 @@
         <v>77</v>
       </c>
       <c r="D83" t="s">
-        <v>3940</v>
+        <v>3922</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>3849</v>
+        <v>3831</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>3850</v>
+        <v>3832</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J83" s="15" t="s">
-        <v>3851</v>
+        <v>3833</v>
       </c>
     </row>
     <row r="84" spans="2:12">
@@ -15580,25 +15605,25 @@
         <v>78</v>
       </c>
       <c r="D84" t="s">
-        <v>3942</v>
+        <v>3924</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>3739</v>
+        <v>3721</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H84" s="15" t="s">
-        <v>3943</v>
+        <v>3925</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J84" s="15" t="s">
-        <v>3945</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="85" spans="2:12">
@@ -15609,25 +15634,25 @@
         <v>79</v>
       </c>
       <c r="D85" t="s">
-        <v>3944</v>
+        <v>3926</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>3946</v>
+        <v>3928</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H85" s="15" t="s">
-        <v>3744</v>
+        <v>3726</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J85" s="15" t="s">
-        <v>3746</v>
+        <v>3728</v>
       </c>
     </row>
     <row r="86" spans="2:12">
@@ -15638,25 +15663,25 @@
         <v>80</v>
       </c>
       <c r="D86" t="s">
-        <v>3947</v>
+        <v>3929</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>3747</v>
+        <v>3729</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H86" s="15" t="s">
-        <v>3748</v>
+        <v>3730</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J86" s="15" t="s">
-        <v>3749</v>
+        <v>3731</v>
       </c>
     </row>
     <row r="87" spans="2:12">
@@ -15667,25 +15692,25 @@
         <v>81</v>
       </c>
       <c r="D87" t="s">
-        <v>3948</v>
+        <v>3930</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F87" s="15" t="s">
-        <v>3750</v>
+        <v>3732</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>3751</v>
+        <v>3733</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J87" s="15" t="s">
-        <v>3753</v>
+        <v>3735</v>
       </c>
     </row>
     <row r="88" spans="2:12">
@@ -15696,25 +15721,25 @@
         <v>82</v>
       </c>
       <c r="D88" t="s">
-        <v>3949</v>
+        <v>3931</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F88" s="15" t="s">
-        <v>3754</v>
+        <v>3736</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>3755</v>
+        <v>3737</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J88" s="15" t="s">
-        <v>3756</v>
+        <v>3738</v>
       </c>
     </row>
     <row r="89" spans="2:12">
@@ -15725,19 +15750,19 @@
         <v>83</v>
       </c>
       <c r="D89" t="s">
-        <v>3950</v>
+        <v>3932</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F89" s="15" t="s">
-        <v>3757</v>
+        <v>3739</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H89" s="15" t="s">
-        <v>3758</v>
+        <v>3740</v>
       </c>
     </row>
     <row r="90" spans="2:12">
@@ -15748,13 +15773,13 @@
         <v>84</v>
       </c>
       <c r="D90" t="s">
-        <v>3951</v>
+        <v>3933</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="F90" s="15" t="s">
-        <v>3759</v>
+        <v>3741</v>
       </c>
     </row>
     <row r="91" spans="2:12">
@@ -15765,25 +15790,25 @@
         <v>85</v>
       </c>
       <c r="D91" t="s">
-        <v>3952</v>
+        <v>3934</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F91" s="15" t="s">
-        <v>3760</v>
+        <v>3742</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H91" s="15" t="s">
-        <v>3762</v>
+        <v>3744</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J91" s="15" t="s">
-        <v>3764</v>
+        <v>3746</v>
       </c>
     </row>
     <row r="92" spans="2:12">
@@ -15794,25 +15819,25 @@
         <v>86</v>
       </c>
       <c r="D92" t="s">
-        <v>3953</v>
+        <v>3935</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F92" s="15" t="s">
-        <v>3765</v>
+        <v>3747</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H92" s="15" t="s">
-        <v>3768</v>
+        <v>3750</v>
       </c>
       <c r="I92" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J92" s="15" t="s">
-        <v>3954</v>
+        <v>3936</v>
       </c>
     </row>
     <row r="93" spans="2:12">
@@ -15823,25 +15848,25 @@
         <v>87</v>
       </c>
       <c r="D93" t="s">
-        <v>3955</v>
+        <v>3937</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F93" s="15" t="s">
-        <v>3769</v>
+        <v>3751</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H93" s="15" t="s">
-        <v>3956</v>
+        <v>3938</v>
       </c>
       <c r="I93" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J93" s="15" t="s">
-        <v>3770</v>
+        <v>3752</v>
       </c>
     </row>
     <row r="94" spans="2:12">
@@ -15852,25 +15877,25 @@
         <v>88</v>
       </c>
       <c r="D94" t="s">
-        <v>3957</v>
+        <v>3939</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F94" s="15" t="s">
-        <v>3771</v>
+        <v>3753</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H94" s="15" t="s">
-        <v>3773</v>
+        <v>3755</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J94" s="15" t="s">
-        <v>3958</v>
+        <v>3940</v>
       </c>
     </row>
     <row r="95" spans="2:12">
@@ -15881,25 +15906,25 @@
         <v>89</v>
       </c>
       <c r="D95" t="s">
-        <v>3959</v>
+        <v>3941</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F95" s="15" t="s">
-        <v>3960</v>
+        <v>3942</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H95" s="15" t="s">
-        <v>3961</v>
+        <v>3943</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J95" s="15" t="s">
-        <v>3962</v>
+        <v>3944</v>
       </c>
     </row>
     <row r="96" spans="2:12">
@@ -15910,25 +15935,25 @@
         <v>90</v>
       </c>
       <c r="D96" t="s">
-        <v>3963</v>
+        <v>3945</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F96" s="15" t="s">
-        <v>3964</v>
+        <v>3946</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H96" s="15" t="s">
-        <v>3965</v>
+        <v>3947</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J96" s="15" t="s">
-        <v>3966</v>
+        <v>3948</v>
       </c>
     </row>
     <row r="97" spans="2:10">
@@ -15939,25 +15964,25 @@
         <v>91</v>
       </c>
       <c r="D97" t="s">
-        <v>3967</v>
+        <v>3949</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>2617</v>
       </c>
       <c r="F97" s="15" t="s">
-        <v>3968</v>
+        <v>3950</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>2618</v>
       </c>
       <c r="H97" s="15" t="s">
-        <v>3969</v>
+        <v>3951</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>2619</v>
       </c>
       <c r="J97" s="15" t="s">
-        <v>3970</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="98" spans="2:10">
@@ -15968,7 +15993,7 @@
         <v>92</v>
       </c>
       <c r="D98" t="s">
-        <v>3971</v>
+        <v>3953</v>
       </c>
     </row>
     <row r="99" spans="2:10">
@@ -15979,7 +16004,7 @@
         <v>93</v>
       </c>
       <c r="D99" t="s">
-        <v>3972</v>
+        <v>3954</v>
       </c>
     </row>
     <row r="100" spans="2:10">
@@ -15990,7 +16015,7 @@
         <v>94</v>
       </c>
       <c r="D100" t="s">
-        <v>3973</v>
+        <v>3955</v>
       </c>
     </row>
     <row r="101" spans="2:10">
@@ -16001,7 +16026,7 @@
         <v>95</v>
       </c>
       <c r="D101" t="s">
-        <v>3974</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="102" spans="2:10">

</xml_diff>